<commit_message>
Simulation Lattice Machanism OK starting Energetics
</commit_message>
<xml_diff>
--- a/calc UBI-QEP per Matlab.xlsx
+++ b/calc UBI-QEP per Matlab.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
   <si>
     <t>T [K]</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>UBI-QEP class</t>
+  </si>
+  <si>
+    <t>Pe_Ratio</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -598,11 +601,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -656,6 +685,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -968,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z56"/>
+  <dimension ref="A2:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,14 +1031,14 @@
     <col min="16" max="18" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="5.42578125" customWidth="1"/>
     <col min="20" max="20" width="7.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" ht="45" x14ac:dyDescent="0.25">
       <c r="H2" s="21" t="s">
         <v>23</v>
       </c>
@@ -1041,16 +1082,19 @@
         <v>30</v>
       </c>
       <c r="V2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="W2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="Y2" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>116</v>
       </c>
@@ -1105,22 +1149,26 @@
         <f>R3/$C$9^(T3)*((Rgas*1000*4.184)*T/(2*PI()*MW_H2))^0.5*(T/T0)^S3</f>
         <v>2.1599061825239194E+18</v>
       </c>
-      <c r="V3" s="15">
-        <f t="shared" ref="V3:V40" si="0">U3*EXP(-O3/Rgas/T)</f>
+      <c r="V3" s="49">
+        <f>U3/U4</f>
+        <v>0.14597654828369858</v>
+      </c>
+      <c r="W3" s="15">
+        <f t="shared" ref="W3:W40" si="0">U3*EXP(-O3/Rgas/T)</f>
         <v>2.1599061825239194E+18</v>
       </c>
-      <c r="W3" s="15">
+      <c r="X3" s="15">
         <v>2.159902E+18</v>
       </c>
-      <c r="X3" s="40">
-        <f t="shared" ref="X3:X40" si="1">(ABS(W3)-ABS(V3))/ABS(W3)*100</f>
+      <c r="Y3" s="40">
+        <f t="shared" ref="Y3:Y40" si="1">(ABS(X3)-ABS(W3))/ABS(X3)*100</f>
         <v>-1.9364415234394896E-4</v>
       </c>
-      <c r="Z3" s="39">
+      <c r="AA3" s="39">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="H4" s="11">
         <v>2</v>
       </c>
@@ -1163,22 +1211,23 @@
         <f>R4/$C$9^(T4-1)*(T/T0)^S4</f>
         <v>1.4796254658154013E+19</v>
       </c>
-      <c r="V4" s="15">
+      <c r="V4" s="50"/>
+      <c r="W4" s="15">
         <f t="shared" si="0"/>
         <v>393470074583181.25</v>
       </c>
-      <c r="W4" s="15">
+      <c r="X4" s="15">
         <v>391967000000000</v>
       </c>
-      <c r="X4" s="40">
+      <c r="Y4" s="40">
         <f t="shared" si="1"/>
         <v>-0.38346967555463851</v>
       </c>
-      <c r="Z4" s="42">
+      <c r="AA4" s="42">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
@@ -1237,22 +1286,26 @@
         <f>R5/$C$9^(T5-1)*(T/T0)^S5</f>
         <v>4.7429833235322122E+18</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="51">
+        <f>U5/U6</f>
+        <v>96.075883276423824</v>
+      </c>
+      <c r="W5" s="10">
         <f t="shared" si="0"/>
         <v>41171120787226.508</v>
       </c>
-      <c r="W5" s="10">
+      <c r="X5" s="10">
         <v>41232850000000</v>
       </c>
-      <c r="X5" s="29">
+      <c r="Y5" s="29">
         <f t="shared" si="1"/>
         <v>0.14970881899624253</v>
       </c>
-      <c r="Z5" s="31">
+      <c r="AA5" s="31">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>26</v>
       </c>
@@ -1301,22 +1354,23 @@
         <f>R6/$C$9^(T6-1)*(T/T0)^S6</f>
         <v>4.9367054059612256E+16</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="52"/>
+      <c r="W6" s="10">
         <f t="shared" si="0"/>
         <v>557220014007.96118</v>
       </c>
-      <c r="W6" s="10">
+      <c r="X6" s="10">
         <v>555974200000</v>
       </c>
-      <c r="X6" s="29">
+      <c r="Y6" s="29">
         <f t="shared" si="1"/>
         <v>-0.22407766546742305</v>
       </c>
-      <c r="Z6" s="32">
+      <c r="AA6" s="32">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -1370,22 +1424,26 @@
         <f>R7/$C$9^(T7)*((Rgas*1000*4.184)*T/(2*PI()*MW_H2O))^0.5*(T/T0)^S7</f>
         <v>2798327648.6857262</v>
       </c>
-      <c r="V7" s="15">
+      <c r="V7" s="49">
+        <f t="shared" ref="V7" si="3">U7/U8</f>
+        <v>7.9120839864510776E-4</v>
+      </c>
+      <c r="W7" s="15">
         <f t="shared" si="0"/>
         <v>2798327648.6857262</v>
       </c>
-      <c r="W7" s="15">
+      <c r="X7" s="15">
         <v>2798427000</v>
       </c>
-      <c r="X7" s="27">
+      <c r="Y7" s="27">
         <f t="shared" si="1"/>
         <v>3.5502557070037641E-3</v>
       </c>
-      <c r="Z7" s="33">
+      <c r="AA7" s="33">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="H8" s="11">
         <v>14</v>
       </c>
@@ -1428,19 +1486,20 @@
         <f>R8/$C$9^(T8-1)*(T/T0)^S8</f>
         <v>3536776977440.6816</v>
       </c>
-      <c r="V8" s="15">
+      <c r="V8" s="50"/>
+      <c r="W8" s="15">
         <f t="shared" si="0"/>
         <v>14456366666.686098</v>
       </c>
-      <c r="W8" s="15">
+      <c r="X8" s="15">
         <v>14451570000</v>
       </c>
-      <c r="X8" s="27">
+      <c r="Y8" s="27">
         <f t="shared" si="1"/>
         <v>-3.3191318909281821E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>120</v>
       </c>
@@ -1494,19 +1553,23 @@
         <f>R9/$C$9^(T9)*((Rgas*1000*4.184)*T/(2*PI()*MW_CO))^0.5*(T/T0)^S9</f>
         <v>577796986.68937802</v>
       </c>
-      <c r="V9" s="5">
+      <c r="V9" s="51">
+        <f t="shared" ref="V9" si="4">U9/U10</f>
+        <v>1.5574590551451487E-5</v>
+      </c>
+      <c r="W9" s="5">
         <f t="shared" si="0"/>
         <v>577796986.68937802</v>
       </c>
-      <c r="W9" s="5">
+      <c r="X9" s="5">
         <v>577814100</v>
       </c>
-      <c r="X9" s="27">
+      <c r="Y9" s="27">
         <f t="shared" si="1"/>
         <v>2.9617329556299943E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C10" s="6"/>
       <c r="H10" s="2">
         <v>20</v>
@@ -1550,19 +1613,20 @@
         <f>R10/$C$9^(T10-1)*(T/T0)^S10</f>
         <v>37098695132985.68</v>
       </c>
-      <c r="V10" s="5">
+      <c r="V10" s="52"/>
+      <c r="W10" s="5">
         <f t="shared" si="0"/>
         <v>1650.2758906548002</v>
       </c>
-      <c r="W10" s="5">
+      <c r="X10" s="5">
         <v>1648.326</v>
       </c>
-      <c r="X10" s="27">
+      <c r="Y10" s="27">
         <f t="shared" si="1"/>
         <v>-0.11829520706462973</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
         <v>4</v>
       </c>
@@ -1618,19 +1682,23 @@
         <f>R11/$C$9^(T11)*((Rgas*1000*4.184)*T/(2*PI()*MW_CO2))^0.5*(T/T0)^S11</f>
         <v>247699484.98849353</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="49">
+        <f t="shared" ref="V11" si="5">U11/U12</f>
+        <v>4.158996491330339E-4</v>
+      </c>
+      <c r="W11" s="15">
         <f t="shared" si="0"/>
         <v>247699484.98849353</v>
       </c>
-      <c r="W11" s="15">
+      <c r="X11" s="15">
         <v>247707800</v>
       </c>
-      <c r="X11" s="27">
+      <c r="Y11" s="27">
         <f t="shared" si="1"/>
         <v>3.3567822678446367E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>5</v>
       </c>
@@ -1679,22 +1747,23 @@
         <v>1</v>
       </c>
       <c r="U12" s="11">
-        <f t="shared" ref="U12:U22" si="3">R12/$C$9^(T12-1)*(T/T0)^S12</f>
+        <f t="shared" ref="U12:U22" si="6">R12/$C$9^(T12-1)*(T/T0)^S12</f>
         <v>595575123722.36182</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V12" s="50"/>
+      <c r="W12" s="15">
         <f t="shared" si="0"/>
         <v>68632984621.338882</v>
       </c>
-      <c r="W12" s="15">
+      <c r="X12" s="15">
         <v>68622020000</v>
       </c>
-      <c r="X12" s="27">
+      <c r="Y12" s="27">
         <f t="shared" si="1"/>
         <v>-1.5978284140983384E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>6</v>
       </c>
@@ -1749,22 +1818,26 @@
         <v>2</v>
       </c>
       <c r="U13" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>26525889.500211328</v>
       </c>
-      <c r="V13" s="5">
+      <c r="V13" s="51">
+        <f t="shared" ref="V13" si="7">U13/U14</f>
+        <v>1.1382332172226586</v>
+      </c>
+      <c r="W13" s="5">
         <f t="shared" si="0"/>
         <v>861611.77035165252</v>
       </c>
-      <c r="W13" s="5">
+      <c r="X13" s="5">
         <v>861907.9</v>
       </c>
-      <c r="X13" s="28">
+      <c r="Y13" s="28">
         <f t="shared" si="1"/>
         <v>3.4357458418411251E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>7</v>
       </c>
@@ -1813,22 +1886,23 @@
         <v>2</v>
       </c>
       <c r="U14" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>23304441.566848416</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="52"/>
+      <c r="W14" s="5">
         <f t="shared" si="0"/>
         <v>18.739983769483654</v>
       </c>
-      <c r="W14" s="5">
+      <c r="X14" s="5">
         <v>18.722930000000002</v>
       </c>
-      <c r="X14" s="28">
+      <c r="Y14" s="28">
         <f t="shared" si="1"/>
         <v>-9.1084939609626048E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>25</v>
       </c>
@@ -1883,22 +1957,26 @@
         <v>2</v>
       </c>
       <c r="U15" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.908508756005915E+19</v>
       </c>
-      <c r="V15" s="15">
+      <c r="V15" s="49">
+        <f t="shared" ref="V15" si="8">U15/U16</f>
+        <v>0.52313776999221462</v>
+      </c>
+      <c r="W15" s="15">
         <f t="shared" si="0"/>
         <v>3.7841926668115603E+17</v>
       </c>
-      <c r="W15" s="15">
+      <c r="X15" s="15">
         <v>3.785431E+17</v>
       </c>
-      <c r="X15" s="29">
+      <c r="Y15" s="29">
         <f t="shared" si="1"/>
         <v>3.2713135926653529E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="H16" s="11">
         <v>32</v>
       </c>
@@ -1938,22 +2016,23 @@
         <v>2</v>
       </c>
       <c r="U16" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.5597376500825006E+19</v>
       </c>
-      <c r="V16" s="15">
+      <c r="V16" s="50"/>
+      <c r="W16" s="15">
         <f t="shared" si="0"/>
         <v>791068492677206.75</v>
       </c>
-      <c r="W16" s="15">
+      <c r="X16" s="15">
         <v>790206500000000</v>
       </c>
-      <c r="X16" s="29">
+      <c r="Y16" s="29">
         <f t="shared" si="1"/>
         <v>-0.10908448325934424</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H17" s="2">
         <v>33</v>
       </c>
@@ -1999,22 +2078,26 @@
         <v>2</v>
       </c>
       <c r="U17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.6418685719338134E+17</v>
       </c>
-      <c r="V17" s="5">
+      <c r="V17" s="51">
+        <f t="shared" ref="V17" si="9">U17/U18</f>
+        <v>0.43316725891350455</v>
+      </c>
+      <c r="W17" s="5">
         <f t="shared" si="0"/>
         <v>699499032836.47412</v>
       </c>
-      <c r="W17" s="5">
+      <c r="X17" s="5">
         <v>699522000000</v>
       </c>
-      <c r="X17" s="29">
+      <c r="Y17" s="29">
         <f t="shared" si="1"/>
         <v>3.2832653620442111E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>8</v>
       </c>
@@ -2063,22 +2146,23 @@
         <v>2</v>
       </c>
       <c r="U18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.0989571985664448E+17</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="52"/>
+      <c r="W18" s="5">
         <f t="shared" si="0"/>
         <v>71334492697509.469</v>
       </c>
-      <c r="W18" s="5">
+      <c r="X18" s="5">
         <v>71325160000000</v>
       </c>
-      <c r="X18" s="29">
+      <c r="Y18" s="29">
         <f t="shared" si="1"/>
         <v>-1.3084720047552295E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>9</v>
       </c>
@@ -2132,22 +2216,26 @@
         <v>2</v>
       </c>
       <c r="U19" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.0869041700707672E+17</v>
       </c>
-      <c r="V19" s="15">
+      <c r="V19" s="49">
+        <f t="shared" ref="V19" si="10">U19/U20</f>
+        <v>182.73106149450714</v>
+      </c>
+      <c r="W19" s="15">
         <f t="shared" si="0"/>
         <v>3886743.8141154968</v>
       </c>
-      <c r="W19" s="15">
+      <c r="X19" s="15">
         <v>3891513</v>
       </c>
-      <c r="X19" s="28">
+      <c r="Y19" s="28">
         <f t="shared" si="1"/>
         <v>0.12255351284971121</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
@@ -2198,22 +2286,23 @@
         <v>2</v>
       </c>
       <c r="U20" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>594810844517224.75</v>
       </c>
-      <c r="V20" s="15">
+      <c r="V20" s="50"/>
+      <c r="W20" s="15">
         <f t="shared" si="0"/>
         <v>25290942.690451734</v>
       </c>
-      <c r="W20" s="15">
+      <c r="X20" s="15">
         <v>25263330</v>
       </c>
-      <c r="X20" s="28">
+      <c r="Y20" s="28">
         <f t="shared" si="1"/>
         <v>-0.10929948843534786</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>3</v>
       </c>
@@ -2267,22 +2356,26 @@
         <v>2</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.3611064640152719E+20</v>
       </c>
-      <c r="V21" s="5">
+      <c r="V21" s="51">
+        <f t="shared" ref="V21" si="11">U21/U22</f>
+        <v>235.78837794743731</v>
+      </c>
+      <c r="W21" s="5">
         <f>U21*EXP(-O21/Rgas/T)</f>
         <v>5.3553061479056186E+20</v>
       </c>
-      <c r="W21" s="5">
+      <c r="X21" s="5">
         <v>5.3554430000000002E+20</v>
       </c>
-      <c r="X21" s="28">
+      <c r="Y21" s="28">
         <f t="shared" si="1"/>
         <v>2.5553832686033345E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>2</v>
       </c>
@@ -2330,22 +2423,23 @@
         <v>2</v>
       </c>
       <c r="U22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.6978032248193802E+18</v>
       </c>
-      <c r="V22" s="5">
+      <c r="V22" s="52"/>
+      <c r="W22" s="5">
         <f t="shared" si="0"/>
         <v>6.6856283341004888E+16</v>
       </c>
-      <c r="W22" s="5">
+      <c r="X22" s="5">
         <v>6.661956E+16</v>
       </c>
-      <c r="X22" s="28">
+      <c r="Y22" s="28">
         <f t="shared" si="1"/>
         <v>-0.3553360919899321</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>10</v>
       </c>
@@ -2402,19 +2496,23 @@
         <f>R23/$C$9^(T23)*((Rgas*1000*4.184)*T/(2*PI()*MW_CH4))^0.5*(T/T0)^S23</f>
         <v>4.913743079331207E+17</v>
       </c>
-      <c r="V23" s="15">
+      <c r="V23" s="49">
+        <f t="shared" ref="V23" si="12">U23/U24</f>
+        <v>0.33427056005300726</v>
+      </c>
+      <c r="W23" s="15">
         <f t="shared" si="0"/>
         <v>98055945025626.953</v>
       </c>
-      <c r="W23" s="15">
+      <c r="X23" s="15">
         <v>98186210000000</v>
       </c>
-      <c r="X23" s="30">
+      <c r="Y23" s="30">
         <f t="shared" si="1"/>
         <v>0.13267135412706824</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H24" s="11">
         <v>56</v>
       </c>
@@ -2454,22 +2552,23 @@
         <v>2</v>
       </c>
       <c r="U24" s="11">
-        <f t="shared" ref="U24:U40" si="4">R24/$C$9^(T24-1)*(T/T0)^S24</f>
+        <f t="shared" ref="U24:U40" si="13">R24/$C$9^(T24-1)*(T/T0)^S24</f>
         <v>1.4699897826933983E+18</v>
       </c>
-      <c r="V24" s="15">
+      <c r="V24" s="50"/>
+      <c r="W24" s="15">
         <f t="shared" si="0"/>
         <v>1.593641264842411E+16</v>
       </c>
-      <c r="W24" s="15">
+      <c r="X24" s="15">
         <v>1.590604E+16</v>
       </c>
-      <c r="X24" s="30">
+      <c r="Y24" s="30">
         <f t="shared" si="1"/>
         <v>-0.19095040892711196</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H25" s="2">
         <v>57</v>
       </c>
@@ -2515,22 +2614,26 @@
         <v>2</v>
       </c>
       <c r="U25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.0850268465904686E+18</v>
       </c>
-      <c r="V25" s="5">
+      <c r="V25" s="51">
+        <f t="shared" ref="V25" si="14">U25/U26</f>
+        <v>11.40636308162226</v>
+      </c>
+      <c r="W25" s="5">
         <f t="shared" si="0"/>
         <v>558157091030536.87</v>
       </c>
-      <c r="W25" s="5">
+      <c r="X25" s="5">
         <v>558924700000000</v>
       </c>
-      <c r="X25" s="29">
+      <c r="Y25" s="29">
         <f t="shared" si="1"/>
         <v>0.13733674132904217</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>12</v>
       </c>
@@ -2585,22 +2688,23 @@
         <v>2</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>9.5124698278160688E+16</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="52"/>
+      <c r="W26" s="5">
         <f t="shared" si="0"/>
         <v>1990103390.1965632</v>
       </c>
-      <c r="W26" s="5">
+      <c r="X26" s="5">
         <v>1984949000</v>
       </c>
-      <c r="X26" s="29">
+      <c r="Y26" s="29">
         <f t="shared" si="1"/>
         <v>-0.25967368413814379</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2615,7 +2719,7 @@
         <v>1.5</v>
       </c>
       <c r="E27" s="22">
-        <f t="shared" ref="E27:E38" si="5">C27-D27*Rgas*deltaT</f>
+        <f t="shared" ref="E27:E38" si="15">C27-D27*Rgas*deltaT</f>
         <v>60.889709930688333</v>
       </c>
       <c r="F27" s="23">
@@ -2667,22 +2771,26 @@
         <v>2</v>
       </c>
       <c r="U27" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.950839074190498E+18</v>
       </c>
-      <c r="V27" s="15">
+      <c r="V27" s="49">
+        <f t="shared" ref="V27" si="16">U27/U28</f>
+        <v>5.9012564102332545</v>
+      </c>
+      <c r="W27" s="15">
         <f t="shared" si="0"/>
         <v>1951779691116.3884</v>
       </c>
-      <c r="W27" s="15">
+      <c r="X27" s="15">
         <v>1953577000000</v>
       </c>
-      <c r="X27" s="29">
+      <c r="Y27" s="29">
         <f t="shared" si="1"/>
         <v>9.2000923619164857E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2697,7 +2805,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>68.119613240917786</v>
       </c>
       <c r="F28" s="23">
@@ -2743,22 +2851,23 @@
         <v>2</v>
       </c>
       <c r="U28" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>3.305802931741088E+17</v>
       </c>
-      <c r="V28" s="15">
+      <c r="V28" s="50"/>
+      <c r="W28" s="15">
         <f t="shared" si="0"/>
         <v>196028256863.89966</v>
       </c>
-      <c r="W28" s="15">
+      <c r="X28" s="15">
         <v>195582600000</v>
       </c>
-      <c r="X28" s="29">
+      <c r="Y28" s="29">
         <f t="shared" si="1"/>
         <v>-0.22786120232559451</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2773,7 +2882,7 @@
         <v>2.5</v>
       </c>
       <c r="E29" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>8.4495165511472283</v>
       </c>
       <c r="F29" s="23">
@@ -2825,22 +2934,26 @@
         <v>2</v>
       </c>
       <c r="U29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.4566681267122695E+20</v>
       </c>
-      <c r="V29" s="5">
+      <c r="V29" s="51">
+        <f t="shared" ref="V29" si="17">U29/U30</f>
+        <v>13.176436022951423</v>
+      </c>
+      <c r="W29" s="5">
         <f t="shared" si="0"/>
         <v>1393244934660.1694</v>
       </c>
-      <c r="W29" s="5">
+      <c r="X29" s="5">
         <v>1393787000000</v>
       </c>
-      <c r="X29" s="29">
+      <c r="Y29" s="29">
         <f t="shared" si="1"/>
         <v>3.8891547979035997E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2855,7 +2968,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>36.619613240917779</v>
       </c>
       <c r="F30" s="23">
@@ -2901,22 +3014,23 @@
         <v>2</v>
       </c>
       <c r="U30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.1055099604892908E+19</v>
       </c>
-      <c r="V30" s="5">
+      <c r="V30" s="52"/>
+      <c r="W30" s="5">
         <f t="shared" si="0"/>
         <v>444035923515434.69</v>
       </c>
-      <c r="W30" s="5">
+      <c r="X30" s="5">
         <v>443253200000000</v>
       </c>
-      <c r="X30" s="29">
+      <c r="Y30" s="29">
         <f t="shared" si="1"/>
         <v>-0.17658609468238187</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -2930,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>3.3196132409177821</v>
       </c>
       <c r="F31" s="23">
@@ -2982,22 +3096,26 @@
         <v>2</v>
       </c>
       <c r="U31" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>9.924956281535146E+18</v>
       </c>
-      <c r="V31" s="15">
+      <c r="V31" s="49">
+        <f t="shared" ref="V31" si="18">U31/U32</f>
+        <v>6.1044633081730737</v>
+      </c>
+      <c r="W31" s="15">
         <f t="shared" si="0"/>
         <v>1.1191755633102914E+17</v>
       </c>
-      <c r="W31" s="15">
+      <c r="X31" s="15">
         <v>1.119075E+17</v>
       </c>
-      <c r="X31" s="28">
+      <c r="Y31" s="28">
         <f t="shared" si="1"/>
         <v>-8.9862887019511641E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -3011,7 +3129,7 @@
         <v>1.5</v>
       </c>
       <c r="E32" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>157.58970993068834</v>
       </c>
       <c r="F32" s="23">
@@ -3057,22 +3175,23 @@
         <v>2</v>
       </c>
       <c r="U32" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.6258523936489116E+18</v>
       </c>
-      <c r="V32" s="15">
+      <c r="V32" s="50"/>
+      <c r="W32" s="15">
         <f t="shared" si="0"/>
         <v>248439031.37872487</v>
       </c>
-      <c r="W32" s="15">
+      <c r="X32" s="15">
         <v>248135900</v>
       </c>
-      <c r="X32" s="28">
+      <c r="Y32" s="28">
         <f t="shared" si="1"/>
         <v>-0.12216345104633108</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -3086,7 +3205,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>149.31961324091776</v>
       </c>
       <c r="F33" s="23">
@@ -3138,22 +3257,26 @@
         <v>2</v>
       </c>
       <c r="U33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.1630643844841764E+18</v>
       </c>
-      <c r="V33" s="5">
+      <c r="V33" s="51">
+        <f t="shared" ref="V33" si="19">U33/U34</f>
+        <v>8.4120595365195232</v>
+      </c>
+      <c r="W33" s="5">
         <f t="shared" si="0"/>
         <v>1771686311191.3979</v>
       </c>
-      <c r="W33" s="5">
+      <c r="X33" s="5">
         <v>1770763000000</v>
       </c>
-      <c r="X33" s="28">
+      <c r="Y33" s="28">
         <f t="shared" si="1"/>
         <v>-5.2141997059908601E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -3167,7 +3290,7 @@
         <v>2.5</v>
       </c>
       <c r="E34" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>106.94951655114723</v>
       </c>
       <c r="F34" s="23">
@@ -3213,22 +3336,23 @@
         <v>2</v>
       </c>
       <c r="U34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.3826154931915669E+17</v>
       </c>
-      <c r="V34" s="5">
+      <c r="V34" s="52"/>
+      <c r="W34" s="5">
         <f t="shared" si="0"/>
         <v>6733897633168181</v>
       </c>
-      <c r="W34" s="5">
+      <c r="X34" s="5">
         <v>6731945000000000</v>
       </c>
-      <c r="X34" s="28">
+      <c r="Y34" s="28">
         <f t="shared" si="1"/>
         <v>-2.900548308372989E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -3242,7 +3366,7 @@
         <v>2.5</v>
       </c>
       <c r="E35" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>40.049516551147228</v>
       </c>
       <c r="F35" s="23">
@@ -3294,22 +3418,26 @@
         <v>2</v>
       </c>
       <c r="U35" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>1.6185172285848158E+19</v>
       </c>
-      <c r="V35" s="15">
+      <c r="V35" s="49">
+        <f t="shared" ref="V35" si="20">U35/U36</f>
+        <v>16.250544973287912</v>
+      </c>
+      <c r="W35" s="15">
         <f t="shared" si="0"/>
         <v>14343775327962.777</v>
       </c>
-      <c r="W35" s="15">
+      <c r="X35" s="15">
         <v>14338250000000</v>
       </c>
-      <c r="X35" s="28">
+      <c r="Y35" s="28">
         <f t="shared" si="1"/>
         <v>-3.8535581139799796E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -3323,7 +3451,7 @@
         <v>2.5</v>
       </c>
       <c r="E36" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>59.849516551147232</v>
       </c>
       <c r="F36" s="23">
@@ -3369,22 +3497,23 @@
         <v>2</v>
       </c>
       <c r="U36" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>9.959772003002231E+17</v>
       </c>
-      <c r="V36" s="15">
+      <c r="V36" s="50"/>
+      <c r="W36" s="15">
         <f t="shared" si="0"/>
         <v>1936473590643.5566</v>
       </c>
-      <c r="W36" s="15">
+      <c r="X36" s="15">
         <v>1934683000000</v>
       </c>
-      <c r="X36" s="28">
+      <c r="Y36" s="28">
         <f t="shared" si="1"/>
         <v>-9.2552146452759484E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -3398,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>4.1196132409177819</v>
       </c>
       <c r="F37" s="23">
@@ -3450,22 +3579,26 @@
         <v>2</v>
       </c>
       <c r="U37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>2.7086574726675624E+19</v>
       </c>
-      <c r="V37" s="5">
+      <c r="V37" s="51">
+        <f t="shared" ref="V37" si="21">U37/U38</f>
+        <v>7.2860120654657541</v>
+      </c>
+      <c r="W37" s="5">
         <f t="shared" si="0"/>
         <v>376243314096700.75</v>
       </c>
-      <c r="W37" s="5">
+      <c r="X37" s="5">
         <v>376264600000000</v>
       </c>
-      <c r="X37" s="28">
+      <c r="Y37" s="28">
         <f t="shared" si="1"/>
         <v>5.6571634161837175E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12</v>
       </c>
@@ -3480,7 +3613,7 @@
         <v>1.5</v>
       </c>
       <c r="E38" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>98.589709930688343</v>
       </c>
       <c r="F38" s="23">
@@ -3526,22 +3659,23 @@
         <v>2</v>
       </c>
       <c r="U38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>3.7176132132776161E+18</v>
       </c>
-      <c r="V38" s="5">
+      <c r="V38" s="52"/>
+      <c r="W38" s="5">
         <f t="shared" si="0"/>
         <v>15989641113.89776</v>
       </c>
-      <c r="W38" s="5">
+      <c r="X38" s="5">
         <v>15965260000</v>
       </c>
-      <c r="X38" s="28">
+      <c r="Y38" s="28">
         <f t="shared" si="1"/>
         <v>-0.15271354113719657</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H39" s="11">
         <v>79</v>
       </c>
@@ -3587,22 +3721,26 @@
         <v>2</v>
       </c>
       <c r="U39" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>6.2621434765029663E+19</v>
       </c>
-      <c r="V39" s="15">
+      <c r="V39" s="49">
+        <f t="shared" ref="V39" si="22">U39/U40</f>
+        <v>0.27111223812444885</v>
+      </c>
+      <c r="W39" s="15">
         <f t="shared" si="0"/>
         <v>22127632338.301205</v>
       </c>
-      <c r="W39" s="15">
+      <c r="X39" s="15">
         <v>22152010000</v>
       </c>
-      <c r="X39" s="28">
+      <c r="Y39" s="28">
         <f t="shared" si="1"/>
         <v>0.11004717720331164</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H40" s="11">
         <v>80</v>
       </c>
@@ -3642,24 +3780,25 @@
         <v>2</v>
       </c>
       <c r="U40" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="13"/>
         <v>2.3097974181558157E+20</v>
       </c>
-      <c r="V40" s="15">
+      <c r="V40" s="50"/>
+      <c r="W40" s="15">
         <f t="shared" si="0"/>
         <v>2.9580744067821614E+18</v>
       </c>
-      <c r="W40" s="15">
+      <c r="X40" s="15">
         <v>2.94969E+18</v>
       </c>
-      <c r="X40" s="28">
+      <c r="Y40" s="28">
         <f t="shared" si="1"/>
         <v>-0.28424704908520582</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="P42" s="38"/>
-      <c r="W42" s="38"/>
+      <c r="X42" s="38"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
@@ -3671,6 +3810,27 @@
       <c r="A56" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="V15:V16"/>
+    <mergeCell ref="V17:V18"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="V31:V32"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="V35:V36"/>
+    <mergeCell ref="V37:V38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3705,12 +3865,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
@@ -4994,7 +5154,7 @@
     <row r="34" spans="20:20" x14ac:dyDescent="0.3">
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="20:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T35" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean code with 4 input of Zacros ok
</commit_message>
<xml_diff>
--- a/calc UBI-QEP per Matlab.xlsx
+++ b/calc UBI-QEP per Matlab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="-165" windowWidth="14430" windowHeight="12795"/>
+    <workbookView xWindow="885" yWindow="-165" windowWidth="14430" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
   <si>
     <t>T [K]</t>
   </si>
@@ -454,13 +454,32 @@
   <si>
     <t>Pe_Ratio</t>
   </si>
+  <si>
+    <t>rif</t>
+  </si>
+  <si>
+    <t>H_RIF</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>energetics [eV]</t>
+  </si>
+  <si>
+    <t>energetics [kacl/mol]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -631,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -681,10 +700,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -700,6 +720,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1146,7 @@
       <c r="N3" s="15">
         <v>0</v>
       </c>
-      <c r="O3" s="47">
+      <c r="O3" s="46">
         <f>MAX(0,L3,N3)</f>
         <v>0</v>
       </c>
@@ -1149,7 +1170,7 @@
         <f>R3/$C$9^(T3)*((Rgas*1000*4.184)*T/(2*PI()*MW_H2))^0.5*(T/T0)^S3</f>
         <v>2.1599061825239194E+18</v>
       </c>
-      <c r="V3" s="49">
+      <c r="V3" s="50">
         <f>U3/U4</f>
         <v>0.14597654828369858</v>
       </c>
@@ -1187,7 +1208,7 @@
         <f>N3-L3</f>
         <v>16.184961930558785</v>
       </c>
-      <c r="O4" s="47">
+      <c r="O4" s="46">
         <f>O3-L3</f>
         <v>16.184961930558785</v>
       </c>
@@ -1211,7 +1232,7 @@
         <f>R4/$C$9^(T4-1)*(T/T0)^S4</f>
         <v>1.4796254658154013E+19</v>
       </c>
-      <c r="V4" s="50"/>
+      <c r="V4" s="51"/>
       <c r="W4" s="15">
         <f t="shared" si="0"/>
         <v>393470074583181.25</v>
@@ -1262,7 +1283,7 @@
         <f>M5*(L5+(Q_H*Q_OH)/(Q_H+Q_OH))</f>
         <v>17.904966325343334</v>
       </c>
-      <c r="O5" s="48">
+      <c r="O5" s="47">
         <f>MAX(0,L5,N5)</f>
         <v>17.904966325343334</v>
       </c>
@@ -1286,7 +1307,7 @@
         <f>R5/$C$9^(T5-1)*(T/T0)^S5</f>
         <v>4.7429833235322122E+18</v>
       </c>
-      <c r="V5" s="51">
+      <c r="V5" s="52">
         <f>U5/U6</f>
         <v>96.075883276423824</v>
       </c>
@@ -1330,7 +1351,7 @@
         <f>N5-L5</f>
         <v>17.501518850912973</v>
       </c>
-      <c r="O6" s="48">
+      <c r="O6" s="47">
         <f>O5-L5</f>
         <v>17.501518850912973</v>
       </c>
@@ -1354,7 +1375,7 @@
         <f>R6/$C$9^(T6-1)*(T/T0)^S6</f>
         <v>4.9367054059612256E+16</v>
       </c>
-      <c r="V6" s="52"/>
+      <c r="V6" s="53"/>
       <c r="W6" s="10">
         <f t="shared" si="0"/>
         <v>557220014007.96118</v>
@@ -1400,7 +1421,7 @@
       <c r="N7" s="15">
         <v>0</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="46">
         <f>MAX(0,L7,N7)</f>
         <v>0</v>
       </c>
@@ -1424,7 +1445,7 @@
         <f>R7/$C$9^(T7)*((Rgas*1000*4.184)*T/(2*PI()*MW_H2O))^0.5*(T/T0)^S7</f>
         <v>2798327648.6857262</v>
       </c>
-      <c r="V7" s="49">
+      <c r="V7" s="50">
         <f t="shared" ref="V7" si="3">U7/U8</f>
         <v>7.9120839864510776E-4</v>
       </c>
@@ -1462,7 +1483,7 @@
         <f>N7-L7</f>
         <v>8.4495165511472283</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="46">
         <f>O7-L7</f>
         <v>8.4495165511472283</v>
       </c>
@@ -1486,7 +1507,7 @@
         <f>R8/$C$9^(T8-1)*(T/T0)^S8</f>
         <v>3536776977440.6816</v>
       </c>
-      <c r="V8" s="50"/>
+      <c r="V8" s="51"/>
       <c r="W8" s="15">
         <f t="shared" si="0"/>
         <v>14456366666.686098</v>
@@ -1529,7 +1550,7 @@
       <c r="N9" s="5">
         <v>0</v>
       </c>
-      <c r="O9" s="46">
+      <c r="O9" s="45">
         <f>MAX(0,L9,N9)</f>
         <v>0</v>
       </c>
@@ -1553,7 +1574,7 @@
         <f>R9/$C$9^(T9)*((Rgas*1000*4.184)*T/(2*PI()*MW_CO))^0.5*(T/T0)^S9</f>
         <v>577796986.68937802</v>
       </c>
-      <c r="V9" s="51">
+      <c r="V9" s="52">
         <f t="shared" ref="V9" si="4">U9/U10</f>
         <v>1.5574590551451487E-5</v>
       </c>
@@ -1589,7 +1610,7 @@
         <f>N9-L9</f>
         <v>36.619613240917779</v>
       </c>
-      <c r="O10" s="46">
+      <c r="O10" s="45">
         <f>O9-L9</f>
         <v>36.619613240917779</v>
       </c>
@@ -1613,7 +1634,7 @@
         <f>R10/$C$9^(T10-1)*(T/T0)^S10</f>
         <v>37098695132985.68</v>
       </c>
-      <c r="V10" s="52"/>
+      <c r="V10" s="53"/>
       <c r="W10" s="5">
         <f t="shared" si="0"/>
         <v>1650.2758906548002</v>
@@ -1658,7 +1679,7 @@
       <c r="N11" s="15">
         <v>0</v>
       </c>
-      <c r="O11" s="47">
+      <c r="O11" s="46">
         <f>MAX(0,L11,N11)</f>
         <v>0</v>
       </c>
@@ -1682,7 +1703,7 @@
         <f>R11/$C$9^(T11)*((Rgas*1000*4.184)*T/(2*PI()*MW_CO2))^0.5*(T/T0)^S11</f>
         <v>247699484.98849353</v>
       </c>
-      <c r="V11" s="49">
+      <c r="V11" s="50">
         <f t="shared" ref="V11" si="5">U11/U12</f>
         <v>4.158996491330339E-4</v>
       </c>
@@ -1726,7 +1747,7 @@
         <f>N11-L11</f>
         <v>3.3196132409177821</v>
       </c>
-      <c r="O12" s="47">
+      <c r="O12" s="46">
         <f>O11-L11</f>
         <v>3.3196132409177821</v>
       </c>
@@ -1750,7 +1771,7 @@
         <f t="shared" ref="U12:U22" si="6">R12/$C$9^(T12-1)*(T/T0)^S12</f>
         <v>595575123722.36182</v>
       </c>
-      <c r="V12" s="50"/>
+      <c r="V12" s="51"/>
       <c r="W12" s="15">
         <f t="shared" si="0"/>
         <v>68632984621.338882</v>
@@ -1797,7 +1818,7 @@
         <f>M13*(L13+(Q_CO*Q_OH)/(Q_CO+Q_OH))</f>
         <v>5.2650839050768905</v>
       </c>
-      <c r="O13" s="48">
+      <c r="O13" s="47">
         <f>MAX(0,L13,N13)</f>
         <v>5.2650839050768905</v>
       </c>
@@ -1821,7 +1842,7 @@
         <f t="shared" si="6"/>
         <v>26525889.500211328</v>
       </c>
-      <c r="V13" s="51">
+      <c r="V13" s="52">
         <f t="shared" ref="V13" si="7">U13/U14</f>
         <v>1.1382332172226586</v>
       </c>
@@ -1865,7 +1886,7 @@
         <f>N13-L13</f>
         <v>21.559960077237839</v>
       </c>
-      <c r="O14" s="48">
+      <c r="O14" s="47">
         <f>O13-L13</f>
         <v>21.559960077237839</v>
       </c>
@@ -1889,7 +1910,7 @@
         <f t="shared" si="6"/>
         <v>23304441.566848416</v>
       </c>
-      <c r="V14" s="52"/>
+      <c r="V14" s="53"/>
       <c r="W14" s="5">
         <f t="shared" si="0"/>
         <v>18.739983769483654</v>
@@ -1936,7 +1957,7 @@
         <f>M15*(L15+(Q_CO*Q_OH)/(Q_CO+Q_OH))</f>
         <v>6.6706742721375925</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="46">
         <f>MAX(0,L15,N15)</f>
         <v>6.6706742721375925</v>
       </c>
@@ -1960,7 +1981,7 @@
         <f t="shared" si="6"/>
         <v>2.908508756005915E+19</v>
       </c>
-      <c r="V15" s="49">
+      <c r="V15" s="50">
         <f t="shared" ref="V15" si="8">U15/U16</f>
         <v>0.52313776999221462</v>
       </c>
@@ -1995,7 +2016,7 @@
         <f>N15-L15</f>
         <v>17.145750335847485</v>
       </c>
-      <c r="O16" s="47">
+      <c r="O16" s="46">
         <f>O15-L15</f>
         <v>17.145750335847485</v>
       </c>
@@ -2019,7 +2040,7 @@
         <f t="shared" si="6"/>
         <v>5.5597376500825006E+19</v>
       </c>
-      <c r="V16" s="50"/>
+      <c r="V16" s="51"/>
       <c r="W16" s="15">
         <f t="shared" si="0"/>
         <v>791068492677206.75</v>
@@ -2057,7 +2078,7 @@
         <f>M17*(L17+(Q_CO2*Q_H)/(Q_CO2+Q_H))</f>
         <v>19.729137555751574</v>
       </c>
-      <c r="O17" s="48">
+      <c r="O17" s="47">
         <f>MAX(0,L17,N17)</f>
         <v>19.729137555751574</v>
       </c>
@@ -2081,7 +2102,7 @@
         <f t="shared" si="6"/>
         <v>2.6418685719338134E+17</v>
       </c>
-      <c r="V17" s="51">
+      <c r="V17" s="52">
         <f t="shared" ref="V17" si="9">U17/U18</f>
         <v>0.43316725891350455</v>
       </c>
@@ -2125,7 +2146,7 @@
         <f>N17-L17</f>
         <v>13.909337447300519</v>
       </c>
-      <c r="O18" s="48">
+      <c r="O18" s="47">
         <f>O17-L17</f>
         <v>13.909337447300519</v>
       </c>
@@ -2149,7 +2170,7 @@
         <f t="shared" si="6"/>
         <v>6.0989571985664448E+17</v>
       </c>
-      <c r="V18" s="52"/>
+      <c r="V18" s="53"/>
       <c r="W18" s="5">
         <f t="shared" si="0"/>
         <v>71334492697509.469</v>
@@ -2195,7 +2216,7 @@
         <f>M19*(L19+(Q_COOH*Q_H)/(Q_COOH+Q_H))</f>
         <v>36.954980809546349</v>
       </c>
-      <c r="O19" s="47">
+      <c r="O19" s="46">
         <f>MAX(0,L19,N19)</f>
         <v>36.954980809546349</v>
       </c>
@@ -2219,7 +2240,7 @@
         <f t="shared" si="6"/>
         <v>1.0869041700707672E+17</v>
       </c>
-      <c r="V19" s="49">
+      <c r="V19" s="50">
         <f t="shared" ref="V19" si="10">U19/U20</f>
         <v>182.73106149450714</v>
       </c>
@@ -2265,7 +2286,7 @@
         <f>N19-L19</f>
         <v>26.076457271406085</v>
       </c>
-      <c r="O20" s="47">
+      <c r="O20" s="46">
         <f>O19-L19</f>
         <v>26.076457271406085</v>
       </c>
@@ -2289,7 +2310,7 @@
         <f t="shared" si="6"/>
         <v>594810844517224.75</v>
       </c>
-      <c r="V20" s="50"/>
+      <c r="V20" s="51"/>
       <c r="W20" s="15">
         <f t="shared" si="0"/>
         <v>25290942.690451734</v>
@@ -2335,7 +2356,7 @@
         <f>M21*(L21+(Q_COOH*Q_OH)/(Q_COOH+Q_OH))</f>
         <v>0.26442314583179172</v>
       </c>
-      <c r="O21" s="48">
+      <c r="O21" s="47">
         <f>MAX(0,L21,N21)</f>
         <v>0.26442314583179172</v>
       </c>
@@ -2359,7 +2380,7 @@
         <f t="shared" si="6"/>
         <v>6.3611064640152719E+20</v>
       </c>
-      <c r="V21" s="51">
+      <c r="V21" s="52">
         <f t="shared" ref="V21" si="11">U21/U22</f>
         <v>235.78837794743731</v>
       </c>
@@ -2402,7 +2423,7 @@
         <f>N21-L21</f>
         <v>5.6807757798524889</v>
       </c>
-      <c r="O22" s="48">
+      <c r="O22" s="47">
         <f>O21-L21</f>
         <v>5.6807757798524889</v>
       </c>
@@ -2426,7 +2447,7 @@
         <f t="shared" si="6"/>
         <v>2.6978032248193802E+18</v>
       </c>
-      <c r="V22" s="52"/>
+      <c r="V22" s="53"/>
       <c r="W22" s="5">
         <f t="shared" si="0"/>
         <v>6.6856283341004888E+16</v>
@@ -2472,7 +2493,7 @@
         <f>M23*(L23-Q_CH4+(Q_CH3*Q_H)/(Q_CH3+Q_H))</f>
         <v>13.088573024654107</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O23" s="46">
         <f>MAX(0,L23,N23)</f>
         <v>13.088573024654107</v>
       </c>
@@ -2496,7 +2517,7 @@
         <f>R23/$C$9^(T23)*((Rgas*1000*4.184)*T/(2*PI()*MW_CH4))^0.5*(T/T0)^S23</f>
         <v>4.913743079331207E+17</v>
       </c>
-      <c r="V23" s="49">
+      <c r="V23" s="50">
         <f t="shared" ref="V23" si="12">U23/U24</f>
         <v>0.33427056005300726</v>
       </c>
@@ -2531,7 +2552,7 @@
         <f>N23-L23</f>
         <v>6.9509392861034378</v>
       </c>
-      <c r="O24" s="47">
+      <c r="O24" s="46">
         <f>O23-L23</f>
         <v>6.9509392861034378</v>
       </c>
@@ -2555,7 +2576,7 @@
         <f t="shared" ref="U24:U40" si="13">R24/$C$9^(T24-1)*(T/T0)^S24</f>
         <v>1.4699897826933983E+18</v>
       </c>
-      <c r="V24" s="50"/>
+      <c r="V24" s="51"/>
       <c r="W24" s="15">
         <f t="shared" si="0"/>
         <v>1.593641264842411E+16</v>
@@ -2593,7 +2614,7 @@
         <f>M25*(L25+(Q_CH2*Q_H)/(Q_CH2+Q_H))</f>
         <v>11.633755803774559</v>
       </c>
-      <c r="O25" s="48">
+      <c r="O25" s="47">
         <f>MAX(0,L25,N25)</f>
         <v>11.633755803774559</v>
       </c>
@@ -2617,7 +2638,7 @@
         <f t="shared" si="13"/>
         <v>1.0850268465904686E+18</v>
       </c>
-      <c r="V25" s="51">
+      <c r="V25" s="52">
         <f t="shared" ref="V25" si="14">U25/U26</f>
         <v>11.40636308162226</v>
       </c>
@@ -2667,7 +2688,7 @@
         <f>N25-L25</f>
         <v>27.166024060150644</v>
       </c>
-      <c r="O26" s="48">
+      <c r="O26" s="47">
         <f>O25-L25</f>
         <v>27.166024060150644</v>
       </c>
@@ -2691,7 +2712,7 @@
         <f t="shared" si="13"/>
         <v>9.5124698278160688E+16</v>
       </c>
-      <c r="V26" s="52"/>
+      <c r="V26" s="53"/>
       <c r="W26" s="5">
         <f t="shared" si="0"/>
         <v>1990103390.1965632</v>
@@ -2750,7 +2771,7 @@
         <f>M27*(L27+(Q_CH*Q_H)/(Q_CH+Q_H))</f>
         <v>21.224325144239888</v>
       </c>
-      <c r="O27" s="47">
+      <c r="O27" s="46">
         <f>MAX(0,L27,N27)</f>
         <v>21.224325144239888</v>
       </c>
@@ -2774,7 +2795,7 @@
         <f t="shared" si="13"/>
         <v>1.950839074190498E+18</v>
       </c>
-      <c r="V27" s="49">
+      <c r="V27" s="50">
         <f t="shared" ref="V27" si="16">U27/U28</f>
         <v>5.9012564102332545</v>
       </c>
@@ -2830,7 +2851,7 @@
         <f>N27-L27</f>
         <v>22.027933128718349</v>
       </c>
-      <c r="O28" s="47">
+      <c r="O28" s="46">
         <f>O27-L27</f>
         <v>22.027933128718349</v>
       </c>
@@ -2854,7 +2875,7 @@
         <f t="shared" si="13"/>
         <v>3.305802931741088E+17</v>
       </c>
-      <c r="V28" s="50"/>
+      <c r="V28" s="51"/>
       <c r="W28" s="15">
         <f t="shared" si="0"/>
         <v>196028256863.89966</v>
@@ -2913,7 +2934,7 @@
         <f>M29*(L29+(Q_C*Q_H)/(Q_C+Q_H))</f>
         <v>28.368478836370691</v>
       </c>
-      <c r="O29" s="48">
+      <c r="O29" s="47">
         <f>MAX(0,L29,N29)</f>
         <v>28.368478836370691</v>
       </c>
@@ -2937,7 +2958,7 @@
         <f t="shared" si="13"/>
         <v>1.4566681267122695E+20</v>
       </c>
-      <c r="V29" s="51">
+      <c r="V29" s="52">
         <f t="shared" ref="V29" si="17">U29/U30</f>
         <v>13.176436022951423</v>
       </c>
@@ -2993,7 +3014,7 @@
         <f>N29-L29</f>
         <v>15.551409507479953</v>
       </c>
-      <c r="O30" s="48">
+      <c r="O30" s="47">
         <f>O29-L29</f>
         <v>15.551409507479953</v>
       </c>
@@ -3017,7 +3038,7 @@
         <f t="shared" si="13"/>
         <v>1.1055099604892908E+19</v>
       </c>
-      <c r="V30" s="52"/>
+      <c r="V30" s="53"/>
       <c r="W30" s="5">
         <f t="shared" si="0"/>
         <v>444035923515434.69</v>
@@ -3075,7 +3096,7 @@
         <f>M31*(L31+(Q_CH2*Q_OH)/(Q_CH2+Q_OH))</f>
         <v>6.8904713162887035</v>
       </c>
-      <c r="O31" s="47">
+      <c r="O31" s="46">
         <f>MAX(0,L31,N31)</f>
         <v>6.8904713162887035</v>
       </c>
@@ -3099,7 +3120,7 @@
         <f t="shared" si="13"/>
         <v>9.924956281535146E+18</v>
       </c>
-      <c r="V31" s="49">
+      <c r="V31" s="50">
         <f t="shared" ref="V31" si="18">U31/U32</f>
         <v>6.1044633081730737</v>
       </c>
@@ -3154,7 +3175,7 @@
         <f>N31-L31</f>
         <v>34.723716818537405</v>
       </c>
-      <c r="O32" s="47">
+      <c r="O32" s="46">
         <f>O31-L31</f>
         <v>34.723716818537405</v>
       </c>
@@ -3178,7 +3199,7 @@
         <f t="shared" si="13"/>
         <v>1.6258523936489116E+18</v>
       </c>
-      <c r="V32" s="50"/>
+      <c r="V32" s="51"/>
       <c r="W32" s="15">
         <f t="shared" si="0"/>
         <v>248439031.37872487</v>
@@ -3236,7 +3257,7 @@
         <f>M33*(L33+(Q_CH3*Q_OH)/(Q_CH3+Q_OH))</f>
         <v>20.57846859692274</v>
       </c>
-      <c r="O33" s="48">
+      <c r="O33" s="47">
         <f>MAX(0,L33,N33)</f>
         <v>20.57846859692274</v>
       </c>
@@ -3260,7 +3281,7 @@
         <f t="shared" si="13"/>
         <v>1.1630643844841764E+18</v>
       </c>
-      <c r="V33" s="51">
+      <c r="V33" s="52">
         <f t="shared" ref="V33" si="19">U33/U34</f>
         <v>8.4120595365195232</v>
       </c>
@@ -3315,7 +3336,7 @@
         <f>N33-L33</f>
         <v>4.6427528661162896</v>
       </c>
-      <c r="O34" s="48">
+      <c r="O34" s="47">
         <f>O33-L33</f>
         <v>4.6427528661162896</v>
       </c>
@@ -3339,7 +3360,7 @@
         <f t="shared" si="13"/>
         <v>1.3826154931915669E+17</v>
       </c>
-      <c r="V34" s="52"/>
+      <c r="V34" s="53"/>
       <c r="W34" s="5">
         <f t="shared" si="0"/>
         <v>6733897633168181</v>
@@ -3397,7 +3418,7 @@
         <f>M35*(L35+(Q_CH2*Q_OH)/(Q_CH2+Q_OH))</f>
         <v>21.410621796867467</v>
       </c>
-      <c r="O35" s="47">
+      <c r="O35" s="46">
         <f>MAX(0,L35,N35)</f>
         <v>21.410621796867467</v>
       </c>
@@ -3421,7 +3442,7 @@
         <f t="shared" si="13"/>
         <v>1.6185172285848158E+19</v>
       </c>
-      <c r="V35" s="49">
+      <c r="V35" s="50">
         <f t="shared" ref="V35" si="20">U35/U36</f>
         <v>16.250544973287912</v>
       </c>
@@ -3476,7 +3497,7 @@
         <f>N35-L35</f>
         <v>20.203566337958641</v>
       </c>
-      <c r="O36" s="47">
+      <c r="O36" s="46">
         <f>O35-L35</f>
         <v>20.203566337958641</v>
       </c>
@@ -3500,7 +3521,7 @@
         <f t="shared" si="13"/>
         <v>9.959772003002231E+17</v>
       </c>
-      <c r="V36" s="50"/>
+      <c r="V36" s="51"/>
       <c r="W36" s="15">
         <f t="shared" si="0"/>
         <v>1936473590643.5566</v>
@@ -3558,7 +3579,7 @@
         <f>M37*(L37+(Q_CH*Q_OH)/(Q_CH+Q_OH))</f>
         <v>17.182699943993562</v>
       </c>
-      <c r="O37" s="48">
+      <c r="O37" s="47">
         <f>MAX(0,L37,N37)</f>
         <v>17.182699943993562</v>
       </c>
@@ -3582,7 +3603,7 @@
         <f t="shared" si="13"/>
         <v>2.7086574726675624E+19</v>
       </c>
-      <c r="V37" s="51">
+      <c r="V37" s="52">
         <f t="shared" ref="V37" si="21">U37/U38</f>
         <v>7.2860120654657541</v>
       </c>
@@ -3638,7 +3659,7 @@
         <f>N37-L37</f>
         <v>29.596321798453907</v>
       </c>
-      <c r="O38" s="48">
+      <c r="O38" s="47">
         <f>O37-L37</f>
         <v>29.596321798453907</v>
       </c>
@@ -3662,7 +3683,7 @@
         <f t="shared" si="13"/>
         <v>3.7176132132776161E+18</v>
       </c>
-      <c r="V38" s="52"/>
+      <c r="V38" s="53"/>
       <c r="W38" s="5">
         <f t="shared" si="0"/>
         <v>15989641113.89776</v>
@@ -3700,7 +3721,7 @@
         <f>M39*(L39+(Q_C*Q_OH)/(Q_C+Q_OH))</f>
         <v>33.4358038137443</v>
       </c>
-      <c r="O39" s="47">
+      <c r="O39" s="46">
         <f>MAX(0,L39,N39)</f>
         <v>33.4358038137443</v>
       </c>
@@ -3724,7 +3745,7 @@
         <f t="shared" si="13"/>
         <v>6.2621434765029663E+19</v>
       </c>
-      <c r="V39" s="49">
+      <c r="V39" s="50">
         <f t="shared" ref="V39" si="22">U39/U40</f>
         <v>0.27111223812444885</v>
       </c>
@@ -3759,7 +3780,7 @@
         <f>N39-L39</f>
         <v>6.6949687010663865</v>
       </c>
-      <c r="O40" s="47">
+      <c r="O40" s="46">
         <f>O39-L39</f>
         <v>6.6949687010663865</v>
       </c>
@@ -3783,7 +3804,7 @@
         <f t="shared" si="13"/>
         <v>2.3097974181558157E+20</v>
       </c>
-      <c r="V40" s="50"/>
+      <c r="V40" s="51"/>
       <c r="W40" s="15">
         <f t="shared" si="0"/>
         <v>2.9580744067821614E+18</v>
@@ -3838,10 +3859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:W35"/>
+  <dimension ref="B1:AF35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,17 +3883,50 @@
     <col min="21" max="21" width="9.140625" customWidth="1"/>
     <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="6">
+        <f>T15</f>
+        <v>-12.287886954821483</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="6">
+        <f>T7</f>
+        <v>3.3242476095640106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B4" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="Z4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="6">
+        <f>T9</f>
+        <v>-53.739054102927511</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>86</v>
       </c>
@@ -3939,8 +3993,26 @@
       <c r="W6" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="AA6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF6" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -4013,8 +4085,37 @@
         <f t="shared" ref="W7:W22" si="5">+U7*Rgas*T</f>
         <v>3.3335557425827491</v>
       </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="48">
+        <f>T11</f>
+        <v>54.459352770190947</v>
+      </c>
+      <c r="AB7" s="48">
+        <f>0.5*AA3</f>
+        <v>1.6621238047820053</v>
+      </c>
+      <c r="AC7" s="48">
+        <f>+AA7-AB7</f>
+        <v>52.797228965408941</v>
+      </c>
+      <c r="AD7">
+        <v>60.889699999999998</v>
+      </c>
+      <c r="AE7" s="48">
+        <f>+AC7-AD7</f>
+        <v>-8.0924710345910569</v>
+      </c>
+      <c r="AF7" s="49">
+        <f>+AE7*0.0433634</f>
+        <v>-0.35091705846138588</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>76</v>
       </c>
@@ -4063,7 +4164,7 @@
       <c r="Q8" s="5">
         <v>-1233.93</v>
       </c>
-      <c r="R8" s="46">
+      <c r="R8" s="45">
         <f t="shared" si="0"/>
         <v>2.3230431127067153</v>
       </c>
@@ -4075,7 +4176,7 @@
         <f t="shared" si="2"/>
         <v>3.5689410483858945</v>
       </c>
-      <c r="U8" s="46">
+      <c r="U8" s="45">
         <f t="shared" si="3"/>
         <v>2.3156579005949167</v>
       </c>
@@ -4087,8 +4188,37 @@
         <f t="shared" si="5"/>
         <v>3.5575949883353237</v>
       </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y8">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA8" s="48">
+        <f>T12</f>
+        <v>12.764847221770795</v>
+      </c>
+      <c r="AB8" s="48">
+        <f>AA4-0.5*AA3</f>
+        <v>-55.401177907709517</v>
+      </c>
+      <c r="AC8" s="48">
+        <f t="shared" ref="AC8:AC17" si="6">+AA8-AB8</f>
+        <v>68.166025129480317</v>
+      </c>
+      <c r="AD8">
+        <v>68.119600000000005</v>
+      </c>
+      <c r="AE8" s="48">
+        <f t="shared" ref="AE8:AE17" si="7">+AC8-AD8</f>
+        <v>4.6425129480311966E-2</v>
+      </c>
+      <c r="AF8" s="49">
+        <f t="shared" ref="AF8:AF17" si="8">+AE8*0.0433634</f>
+        <v>2.0131514597065601E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -4161,8 +4291,37 @@
         <f t="shared" si="5"/>
         <v>-53.732893285772583</v>
       </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="48">
+        <f>T9</f>
+        <v>-53.739054102927511</v>
+      </c>
+      <c r="AB9" s="48">
+        <f>AA4</f>
+        <v>-53.739054102927511</v>
+      </c>
+      <c r="AC9" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>8.4495000000000005</v>
+      </c>
+      <c r="AE9" s="48">
+        <f t="shared" si="7"/>
+        <v>-8.4495000000000005</v>
+      </c>
+      <c r="AF9" s="49">
+        <f t="shared" si="8"/>
+        <v>-0.36639904830000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>77</v>
       </c>
@@ -4211,7 +4370,7 @@
       <c r="Q10" s="5">
         <v>29217.58</v>
       </c>
-      <c r="R10" s="46">
+      <c r="R10" s="45">
         <f t="shared" si="0"/>
         <v>40.334187120180943</v>
       </c>
@@ -4223,7 +4382,7 @@
         <f t="shared" si="2"/>
         <v>61.966278317911346</v>
       </c>
-      <c r="U10" s="46">
+      <c r="U10" s="45">
         <f t="shared" si="3"/>
         <v>40.333786626451058</v>
       </c>
@@ -4235,8 +4394,37 @@
         <f t="shared" si="5"/>
         <v>61.965663030788868</v>
       </c>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="48">
+        <f>T13</f>
+        <v>-22.993262216654838</v>
+      </c>
+      <c r="AB10" s="48">
+        <f>AA2+AA4-3*AA3</f>
+        <v>-75.999683886441034</v>
+      </c>
+      <c r="AC10" s="48">
+        <f t="shared" si="6"/>
+        <v>53.006421669786192</v>
+      </c>
+      <c r="AD10">
+        <v>36.619599999999998</v>
+      </c>
+      <c r="AE10" s="48">
+        <f t="shared" si="7"/>
+        <v>16.386821669786194</v>
+      </c>
+      <c r="AF10" s="49">
+        <f t="shared" si="8"/>
+        <v>0.7105883027956067</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
@@ -4285,7 +4473,7 @@
       <c r="Q11" s="5">
         <v>25473.66</v>
       </c>
-      <c r="R11" s="46">
+      <c r="R11" s="45">
         <f t="shared" si="0"/>
         <v>35.447888508125985</v>
       </c>
@@ -4297,7 +4485,7 @@
         <f t="shared" si="2"/>
         <v>54.459352770190947</v>
       </c>
-      <c r="U11" s="46">
+      <c r="U11" s="45">
         <f t="shared" si="3"/>
         <v>35.447888501835351</v>
       </c>
@@ -4309,8 +4497,37 @@
         <f t="shared" si="5"/>
         <v>54.459352760526507</v>
       </c>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y11">
+        <v>5</v>
+      </c>
+      <c r="Z11" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="48">
+        <f>T14</f>
+        <v>-88.922794903143497</v>
+      </c>
+      <c r="AB11" s="48">
+        <f>AA2+2*AA4-4*AA3</f>
+        <v>-133.06298559893256</v>
+      </c>
+      <c r="AC11" s="48">
+        <f t="shared" si="6"/>
+        <v>44.140190695789059</v>
+      </c>
+      <c r="AD11">
+        <v>3.3195999999999999</v>
+      </c>
+      <c r="AE11" s="48">
+        <f t="shared" si="7"/>
+        <v>40.820590695789058</v>
+      </c>
+      <c r="AF11" s="49">
+        <f t="shared" si="8"/>
+        <v>1.7701196025777794</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
@@ -4359,7 +4576,7 @@
       <c r="Q12" s="5">
         <v>3858.6570000000002</v>
       </c>
-      <c r="R12" s="46">
+      <c r="R12" s="45">
         <f t="shared" si="0"/>
         <v>8.3087083875199426</v>
       </c>
@@ -4371,7 +4588,7 @@
         <f t="shared" si="2"/>
         <v>12.764847221770795</v>
       </c>
-      <c r="U12" s="46">
+      <c r="U12" s="45">
         <f t="shared" si="3"/>
         <v>8.3116075172911632</v>
       </c>
@@ -4383,8 +4600,37 @@
         <f t="shared" si="5"/>
         <v>12.76930121713081</v>
       </c>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y12">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA12" s="48">
+        <f>T19</f>
+        <v>173.64207844444326</v>
+      </c>
+      <c r="AB12" s="48">
+        <f>AA2-2*AA3</f>
+        <v>-18.936382173949504</v>
+      </c>
+      <c r="AC12" s="48">
+        <f t="shared" si="6"/>
+        <v>192.57846061839277</v>
+      </c>
+      <c r="AD12">
+        <v>157.58969999999999</v>
+      </c>
+      <c r="AE12" s="48">
+        <f t="shared" si="7"/>
+        <v>34.988760618392774</v>
+      </c>
+      <c r="AF12" s="49">
+        <f t="shared" si="8"/>
+        <v>1.5172316221996134</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
@@ -4457,8 +4703,37 @@
         <f t="shared" si="5"/>
         <v>-22.991908661109427</v>
       </c>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y13">
+        <v>7</v>
+      </c>
+      <c r="Z13" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA13" s="48">
+        <f>T16</f>
+        <v>146.12455526528456</v>
+      </c>
+      <c r="AB13" s="48">
+        <f>AA2-3/2*AA3</f>
+        <v>-17.274258369167498</v>
+      </c>
+      <c r="AC13" s="48">
+        <f t="shared" si="6"/>
+        <v>163.39881363445204</v>
+      </c>
+      <c r="AD13">
+        <v>149.31960000000001</v>
+      </c>
+      <c r="AE13" s="48">
+        <f t="shared" si="7"/>
+        <v>14.079213634452032</v>
+      </c>
+      <c r="AF13" s="49">
+        <f t="shared" si="8"/>
+        <v>0.61052257251619724</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
@@ -4531,8 +4806,37 @@
         <f t="shared" si="5"/>
         <v>-88.931284665050185</v>
       </c>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y14">
+        <v>8</v>
+      </c>
+      <c r="Z14" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA14" s="48">
+        <f>T17</f>
+        <v>98.127709399495103</v>
+      </c>
+      <c r="AB14" s="48">
+        <f>AA2-AA3</f>
+        <v>-15.612134564385492</v>
+      </c>
+      <c r="AC14" s="48">
+        <f t="shared" si="6"/>
+        <v>113.73984396388059</v>
+      </c>
+      <c r="AD14">
+        <v>106.9495</v>
+      </c>
+      <c r="AE14" s="48">
+        <f t="shared" si="7"/>
+        <v>6.7903439638805878</v>
+      </c>
+      <c r="AF14" s="49">
+        <f t="shared" si="8"/>
+        <v>0.29445240144333951</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -4605,8 +4909,37 @@
         <f t="shared" si="5"/>
         <v>-12.295594219394475</v>
       </c>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>9</v>
+      </c>
+      <c r="Z15" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA15" s="48">
+        <f>T18</f>
+        <v>40.329620495373803</v>
+      </c>
+      <c r="AB15" s="48">
+        <f>AA2-0.5*AA3</f>
+        <v>-13.950010759603488</v>
+      </c>
+      <c r="AC15" s="48">
+        <f t="shared" si="6"/>
+        <v>54.279631254977289</v>
+      </c>
+      <c r="AD15">
+        <v>40.049500000000002</v>
+      </c>
+      <c r="AE15" s="48">
+        <f t="shared" si="7"/>
+        <v>14.230131254977287</v>
+      </c>
+      <c r="AF15" s="49">
+        <f t="shared" si="8"/>
+        <v>0.61706687366208213</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>79</v>
       </c>
@@ -4655,7 +4988,7 @@
       <c r="Q16" s="5">
         <v>71012.44</v>
       </c>
-      <c r="R16" s="46">
+      <c r="R16" s="45">
         <f t="shared" si="0"/>
         <v>95.113266681688089</v>
       </c>
@@ -4667,7 +5000,7 @@
         <f t="shared" si="2"/>
         <v>146.12455526528456</v>
       </c>
-      <c r="U16" s="46">
+      <c r="U16" s="45">
         <f t="shared" si="3"/>
         <v>95.116941331613191</v>
       </c>
@@ -4679,8 +5012,37 @@
         <f t="shared" si="5"/>
         <v>146.13020070892026</v>
       </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y16">
+        <v>10</v>
+      </c>
+      <c r="Z16" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA16" s="48">
+        <f>T21</f>
+        <v>-44.643048861862489</v>
+      </c>
+      <c r="AB16" s="48">
+        <f>AA2+2*AA4-7/2*AA3</f>
+        <v>-131.40086179415056</v>
+      </c>
+      <c r="AC16" s="48">
+        <f t="shared" si="6"/>
+        <v>86.757812932288061</v>
+      </c>
+      <c r="AD16">
+        <v>59.849499999999999</v>
+      </c>
+      <c r="AE16" s="48">
+        <f t="shared" si="7"/>
+        <v>26.908312932288062</v>
+      </c>
+      <c r="AF16" s="49">
+        <f t="shared" si="8"/>
+        <v>1.1668359370079802</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>80</v>
       </c>
@@ -4729,7 +5091,7 @@
       <c r="Q17" s="5">
         <v>46263.6</v>
       </c>
-      <c r="R17" s="46">
+      <c r="R17" s="45">
         <f t="shared" si="0"/>
         <v>63.871859018035344</v>
       </c>
@@ -4741,7 +5103,7 @@
         <f t="shared" si="2"/>
         <v>98.127709399495103</v>
       </c>
-      <c r="U17" s="46">
+      <c r="U17" s="45">
         <f t="shared" si="3"/>
         <v>63.87335897667333</v>
       </c>
@@ -4753,8 +5115,37 @@
         <f t="shared" si="5"/>
         <v>98.130013818179663</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Y17">
+        <v>11</v>
+      </c>
+      <c r="Z17" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA17" s="48">
+        <f>T10</f>
+        <v>61.966278317911346</v>
+      </c>
+      <c r="AB17" s="48">
+        <f>AA4-AA3</f>
+        <v>-57.063301712491523</v>
+      </c>
+      <c r="AC17" s="48">
+        <f t="shared" si="6"/>
+        <v>119.02958003040287</v>
+      </c>
+      <c r="AD17">
+        <v>98.589699999999993</v>
+      </c>
+      <c r="AE17" s="48">
+        <f t="shared" si="7"/>
+        <v>20.439880030402875</v>
+      </c>
+      <c r="AF17" s="49">
+        <f t="shared" si="8"/>
+        <v>0.88634269371037211</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>81</v>
       </c>
@@ -4803,7 +5194,7 @@
       <c r="Q18" s="5">
         <v>16775.580000000002</v>
       </c>
-      <c r="R18" s="46">
+      <c r="R18" s="45">
         <f t="shared" si="0"/>
         <v>26.250769026354529</v>
       </c>
@@ -4815,7 +5206,7 @@
         <f t="shared" si="2"/>
         <v>40.329620495373803</v>
       </c>
-      <c r="U18" s="46">
+      <c r="U18" s="45">
         <f t="shared" si="3"/>
         <v>26.252474118514996</v>
       </c>
@@ -4828,7 +5219,7 @@
         <v>40.332240065096585</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>82</v>
       </c>
@@ -4877,7 +5268,7 @@
       <c r="Q19" s="5">
         <v>85451.3</v>
       </c>
-      <c r="R19" s="46">
+      <c r="R19" s="45">
         <f t="shared" si="0"/>
         <v>113.02457197741518</v>
       </c>
@@ -4889,7 +5280,7 @@
         <f t="shared" si="2"/>
         <v>173.64207844444326</v>
       </c>
-      <c r="U19" s="46">
+      <c r="U19" s="45">
         <f t="shared" si="3"/>
         <v>113.02433639832088</v>
       </c>
@@ -4902,7 +5293,7 @@
         <v>173.6417165192189</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>83</v>
       </c>
@@ -4951,7 +5342,7 @@
       <c r="Q20" s="5">
         <v>-922.79539999999997</v>
       </c>
-      <c r="R20" s="46">
+      <c r="R20" s="45">
         <f t="shared" si="0"/>
         <v>2.2100396385060228</v>
       </c>
@@ -4963,7 +5354,7 @@
         <f t="shared" si="2"/>
         <v>3.3953313829091503</v>
       </c>
-      <c r="U20" s="46">
+      <c r="U20" s="45">
         <f t="shared" si="3"/>
         <v>2.2062124002155503</v>
       </c>
@@ -4976,7 +5367,7 @@
         <v>3.3894515144890986</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>84</v>
       </c>
@@ -5025,7 +5416,7 @@
       <c r="Q21" s="5">
         <v>-27670.86</v>
       </c>
-      <c r="R21" s="46">
+      <c r="R21" s="45">
         <f t="shared" si="0"/>
         <v>-29.058402978015664</v>
       </c>
@@ -5037,7 +5428,7 @@
         <f t="shared" si="2"/>
         <v>-44.643048861862489</v>
       </c>
-      <c r="U21" s="46">
+      <c r="U21" s="45">
         <f t="shared" si="3"/>
         <v>-29.076646621517718</v>
       </c>
@@ -5050,7 +5441,7 @@
         <v>-44.671076963368847</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>85</v>
       </c>
@@ -5099,7 +5490,7 @@
       <c r="Q22" s="5">
         <v>-20491.02</v>
       </c>
-      <c r="R22" s="46">
+      <c r="R22" s="45">
         <f t="shared" si="0"/>
         <v>-19.603168867513887</v>
       </c>
@@ -5111,7 +5502,7 @@
         <f t="shared" si="2"/>
         <v>-30.116769536917126</v>
       </c>
-      <c r="U22" s="46">
+      <c r="U22" s="45">
         <f t="shared" si="3"/>
         <v>-19.531940953252281</v>
       </c>
@@ -5124,28 +5515,28 @@
         <v>-30.007340561790201</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T26" s="6"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T29" s="6"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T30" s="6"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="T32" s="6"/>
     </row>
     <row r="33" spans="20:20" x14ac:dyDescent="0.3">

</xml_diff>